<commit_message>
Modifico el valor de la cochera por mes
Se modifica el valor mensual de la cochera producto del aumento en la
proyaccion
</commit_message>
<xml_diff>
--- a/Valor cochera.xlsx
+++ b/Valor cochera.xlsx
@@ -16,10 +16,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,20 +397,20 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
-        <v>1200</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
         <f>A1*12</f>
-        <v>14400</v>
+        <v>15600</v>
       </c>
       <c r="B2">
         <f>(B3*C3)+(50*12)</f>
@@ -424,7 +420,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="2">
         <f>B2/A2-1</f>
-        <v>0.27499999999999991</v>
+        <v>0.17692307692307696</v>
       </c>
       <c r="B3">
         <v>80</v>

</xml_diff>